<commit_message>
Add new data and update spreadsheet
</commit_message>
<xml_diff>
--- a/Characterisation Data/Array Target Characterisation.xlsx
+++ b/Characterisation Data/Array Target Characterisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/christopher_gardner_stfc_ac_uk/Documents/Coding files/MATLAB/Borghesi Horizontal Laser Positioning/Characterisation Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365.sharepoint.com/sites/TargetFabrication2/Shared Documents/1. Expt Planning/GTA 1022 Borghesi/3. Delivery/Characterisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_FE310490A0B32A38BD8A12762798BD300347D4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F896CFA3-0DE7-4167-9D61-5249CFE4B483}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_FE310490A0B32A38BD8A12762798BD300347D4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C2554E-A47D-4028-9D2B-5C8D0E9DF58A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>Array</t>
   </si>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,16 +266,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>161612</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>185881</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19372</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>357331</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -291,20 +291,62 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="21587408">
-          <a:off x="7381875" y="923612"/>
-          <a:ext cx="3853006" cy="3096260"/>
+          <a:off x="14868525" y="276225"/>
+          <a:ext cx="3853006" cy="4505334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0361C08-1DB1-D57A-456A-1C0C3FB11F61}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7543800" y="381000"/>
+          <a:ext cx="3457575" cy="2790825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -582,10 +624,10 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="4" width="9.140625" style="2"/>
@@ -596,7 +638,7 @@
     <col min="9" max="9" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -625,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -642,7 +684,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="9"/>
       <c r="B3" s="11"/>
       <c r="C3" s="5">
@@ -655,7 +697,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="9"/>
       <c r="B4" s="11"/>
       <c r="C4" s="5">
@@ -668,7 +710,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="9"/>
       <c r="B5" s="12"/>
       <c r="C5" s="5">
@@ -681,7 +723,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="9"/>
       <c r="B6" s="13" t="s">
         <v>10</v>
@@ -696,7 +738,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="9"/>
       <c r="B7" s="11"/>
       <c r="C7" s="5">
@@ -709,7 +751,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="9"/>
       <c r="B8" s="11"/>
       <c r="C8" s="5">
@@ -722,7 +764,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="9"/>
       <c r="B9" s="12"/>
       <c r="C9" s="5">
@@ -735,7 +777,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="9"/>
       <c r="B10" s="13" t="s">
         <v>11</v>
@@ -750,7 +792,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="9"/>
       <c r="B11" s="11"/>
       <c r="C11" s="5">
@@ -769,7 +811,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="5">
@@ -788,7 +830,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="9"/>
       <c r="B13" s="12"/>
       <c r="C13" s="5">
@@ -807,7 +849,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="9"/>
       <c r="B14" s="13" t="s">
         <v>13</v>
@@ -822,7 +864,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="5">
@@ -841,7 +883,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="9"/>
       <c r="B16" s="11"/>
       <c r="C16" s="5">
@@ -854,7 +896,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
       <c r="C17" s="7">
@@ -867,7 +909,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="9">
         <v>2</v>
       </c>
@@ -877,53 +919,85 @@
       <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F18" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="9"/>
       <c r="B19" s="11"/>
       <c r="C19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F19" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="9"/>
       <c r="B20" s="11"/>
       <c r="C20" s="5">
         <v>3</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F20" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="9"/>
       <c r="B21" s="12"/>
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F21" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="9"/>
       <c r="B22" s="13" t="s">
         <v>10</v>
@@ -931,53 +1005,85 @@
       <c r="C22" s="5">
         <v>1</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F22" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="9"/>
       <c r="B23" s="11"/>
       <c r="C23" s="5">
         <v>2</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F23" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="9"/>
       <c r="B24" s="11"/>
       <c r="C24" s="5">
         <v>3</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F24" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="9"/>
       <c r="B25" s="12"/>
       <c r="C25" s="5">
         <v>4</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F25" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" s="9"/>
       <c r="B26" s="13" t="s">
         <v>11</v>
@@ -985,53 +1091,85 @@
       <c r="C26" s="5">
         <v>1</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F26" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="9"/>
       <c r="B27" s="11"/>
       <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F27" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="9"/>
       <c r="B28" s="11"/>
       <c r="C28" s="5">
         <v>3</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F28" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="9"/>
       <c r="B29" s="12"/>
       <c r="C29" s="5">
         <v>4</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F29" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="9"/>
       <c r="B30" s="13" t="s">
         <v>13</v>
@@ -1039,53 +1177,85 @@
       <c r="C30" s="5">
         <v>1</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F30" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="9"/>
       <c r="B31" s="11"/>
       <c r="C31" s="5">
         <v>2</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F31" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="9"/>
       <c r="B32" s="11"/>
       <c r="C32" s="5">
         <v>3</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F32" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="10"/>
       <c r="B33" s="14"/>
       <c r="C33" s="7">
         <v>4</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="5">
+        <f>6</f>
+        <v>6</v>
+      </c>
+      <c r="F33" s="5">
+        <f>300</f>
+        <v>300</v>
+      </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="9">
         <v>3</v>
       </c>
@@ -1102,7 +1272,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="9"/>
       <c r="B35" s="11"/>
       <c r="C35" s="5">
@@ -1115,7 +1285,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="9"/>
       <c r="B36" s="11"/>
       <c r="C36" s="5">
@@ -1128,7 +1298,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="9"/>
       <c r="B37" s="12"/>
       <c r="C37" s="5">
@@ -1141,7 +1311,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="9"/>
       <c r="B38" s="13" t="s">
         <v>10</v>
@@ -1156,7 +1326,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="9"/>
       <c r="B39" s="11"/>
       <c r="C39" s="5">
@@ -1169,7 +1339,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="9"/>
       <c r="B40" s="11"/>
       <c r="C40" s="5">
@@ -1182,7 +1352,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="9"/>
       <c r="B41" s="12"/>
       <c r="C41" s="5">
@@ -1195,7 +1365,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="9"/>
       <c r="B42" s="13" t="s">
         <v>11</v>
@@ -1210,7 +1380,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="9"/>
       <c r="B43" s="11"/>
       <c r="C43" s="5">
@@ -1223,7 +1393,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="9"/>
       <c r="B44" s="11"/>
       <c r="C44" s="5">
@@ -1236,7 +1406,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="9"/>
       <c r="B45" s="12"/>
       <c r="C45" s="5">
@@ -1249,7 +1419,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="9"/>
       <c r="B46" s="13" t="s">
         <v>13</v>
@@ -1264,7 +1434,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="9"/>
       <c r="B47" s="11"/>
       <c r="C47" s="5">
@@ -1277,7 +1447,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="9"/>
       <c r="B48" s="11"/>
       <c r="C48" s="5">
@@ -1290,7 +1460,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="10"/>
       <c r="B49" s="14"/>
       <c r="C49" s="7">
@@ -1303,7 +1473,7 @@
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="9">
         <v>4</v>
       </c>
@@ -1320,7 +1490,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="9"/>
       <c r="B51" s="11"/>
       <c r="C51" s="5">
@@ -1333,7 +1503,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="9"/>
       <c r="B52" s="11"/>
       <c r="C52" s="5">
@@ -1346,7 +1516,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="9"/>
       <c r="B53" s="12"/>
       <c r="C53" s="5">
@@ -1359,7 +1529,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" s="9"/>
       <c r="B54" s="13" t="s">
         <v>10</v>
@@ -1374,7 +1544,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="9"/>
       <c r="B55" s="11"/>
       <c r="C55" s="5">
@@ -1387,7 +1557,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="9"/>
       <c r="B56" s="11"/>
       <c r="C56" s="5">
@@ -1400,7 +1570,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="9"/>
       <c r="B57" s="12"/>
       <c r="C57" s="5">
@@ -1413,7 +1583,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="9"/>
       <c r="B58" s="13" t="s">
         <v>11</v>
@@ -1428,7 +1598,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="9"/>
       <c r="B59" s="11"/>
       <c r="C59" s="5">
@@ -1441,7 +1611,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="9"/>
       <c r="B60" s="11"/>
       <c r="C60" s="5">
@@ -1454,7 +1624,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61" s="9"/>
       <c r="B61" s="12"/>
       <c r="C61" s="5">
@@ -1467,7 +1637,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62" s="9"/>
       <c r="B62" s="13" t="s">
         <v>13</v>
@@ -1482,7 +1652,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63" s="9"/>
       <c r="B63" s="11"/>
       <c r="C63" s="5">
@@ -1495,7 +1665,7 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64" s="9"/>
       <c r="B64" s="11"/>
       <c r="C64" s="5">
@@ -1508,7 +1678,7 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9">
       <c r="A65" s="10"/>
       <c r="B65" s="14"/>
       <c r="C65" s="7">
@@ -1550,15 +1720,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ApprovalRequested xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xsi:nil="true"/>
@@ -1579,7 +1740,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100695ECA461C232F4AAEC38BDBCF991C34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="59a9ea53a97323102fd6db9b998f0b5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xmlns:ns3="029942aa-539e-4767-81e4-a62063a6e1cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1df2dcb4e8f42f9041788b58686dd0b" ns2:_="" ns3:_="">
     <xsd:import namespace="b78d6d24-d6db-4d75-9c62-aa5d16939a2a"/>
@@ -1862,40 +2023,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C55BA5DB-FABC-42B8-A62D-4229D8279EF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDD6B012-B9AC-4751-AE85-9BF9548DF2A7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDD6B012-B9AC-4751-AE85-9BF9548DF2A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b78d6d24-d6db-4d75-9c62-aa5d16939a2a"/>
-    <ds:schemaRef ds:uri="029942aa-539e-4767-81e4-a62063a6e1cb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72F46C54-F7FE-4881-AE33-32A42E9027D0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72F46C54-F7FE-4881-AE33-32A42E9027D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b78d6d24-d6db-4d75-9c62-aa5d16939a2a"/>
-    <ds:schemaRef ds:uri="029942aa-539e-4767-81e4-a62063a6e1cb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C55BA5DB-FABC-42B8-A62D-4229D8279EF7}"/>
 </file>
</xml_diff>

<commit_message>
Add data for Array 4
</commit_message>
<xml_diff>
--- a/Characterisation Data/Array Target Characterisation.xlsx
+++ b/Characterisation Data/Array Target Characterisation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365.sharepoint.com/sites/TargetFabrication2/Shared Documents/1. Expt Planning/GTA 1022 Borghesi/3. Delivery/Characterisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_FE310490A0B32A38BD8A12762798BD300347D4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49EEEC7E-D7DF-4A97-A7FD-BBBD430BD0E9}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_FE310490A0B32A38BD8A12762798BD300347D4B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7C04701-2546-4B10-AFC6-91FC065A0F27}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="15">
   <si>
     <t>Array</t>
   </si>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1595,8 +1595,12 @@
       <c r="C50" s="5">
         <v>1</v>
       </c>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="5">
+        <v>25</v>
+      </c>
       <c r="F50" s="5"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -1608,9 +1612,15 @@
       <c r="C51" s="5">
         <v>2</v>
       </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="5">
+        <v>2</v>
+      </c>
+      <c r="F51" s="5">
+        <v>100</v>
+      </c>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -1621,9 +1631,15 @@
       <c r="C52" s="5">
         <v>3</v>
       </c>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="5">
+        <v>2</v>
+      </c>
+      <c r="F52" s="5">
+        <v>100</v>
+      </c>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -1634,9 +1650,15 @@
       <c r="C53" s="5">
         <v>4</v>
       </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="D53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="5">
+        <v>2</v>
+      </c>
+      <c r="F53" s="5">
+        <v>100</v>
+      </c>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -1649,9 +1671,15 @@
       <c r="C54" s="5">
         <v>1</v>
       </c>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="D54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="5">
+        <v>2</v>
+      </c>
+      <c r="F54" s="5">
+        <v>100</v>
+      </c>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -1662,9 +1690,15 @@
       <c r="C55" s="5">
         <v>2</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="5">
+        <v>2</v>
+      </c>
+      <c r="F55" s="5">
+        <v>100</v>
+      </c>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -1675,9 +1709,15 @@
       <c r="C56" s="5">
         <v>3</v>
       </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="5">
+        <v>2</v>
+      </c>
+      <c r="F56" s="5">
+        <v>100</v>
+      </c>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -1688,9 +1728,15 @@
       <c r="C57" s="5">
         <v>4</v>
       </c>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="5">
+        <v>2</v>
+      </c>
+      <c r="F57" s="5">
+        <v>100</v>
+      </c>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -1703,9 +1749,15 @@
       <c r="C58" s="5">
         <v>1</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="5">
+        <v>2</v>
+      </c>
+      <c r="F58" s="5">
+        <v>100</v>
+      </c>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -1716,9 +1768,15 @@
       <c r="C59" s="5">
         <v>2</v>
       </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="5">
+        <v>2</v>
+      </c>
+      <c r="F59" s="5">
+        <v>100</v>
+      </c>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -1729,9 +1787,15 @@
       <c r="C60" s="5">
         <v>3</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="D60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="5">
+        <v>2</v>
+      </c>
+      <c r="F60" s="5">
+        <v>100</v>
+      </c>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
@@ -1742,9 +1806,15 @@
       <c r="C61" s="5">
         <v>4</v>
       </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="5">
+        <v>2</v>
+      </c>
+      <c r="F61" s="5">
+        <v>100</v>
+      </c>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -1757,9 +1827,15 @@
       <c r="C62" s="5">
         <v>1</v>
       </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="5">
+        <v>2</v>
+      </c>
+      <c r="F62" s="5">
+        <v>100</v>
+      </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -1770,9 +1846,15 @@
       <c r="C63" s="5">
         <v>2</v>
       </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="5">
+        <v>2</v>
+      </c>
+      <c r="F63" s="5">
+        <v>100</v>
+      </c>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
@@ -1783,9 +1865,15 @@
       <c r="C64" s="5">
         <v>3</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" s="5">
+        <v>2</v>
+      </c>
+      <c r="F64" s="5">
+        <v>100</v>
+      </c>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -1796,35 +1884,41 @@
       <c r="C65" s="7">
         <v>4</v>
       </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
+      <c r="D65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="5">
+        <v>2</v>
+      </c>
+      <c r="F65" s="5">
+        <v>100</v>
+      </c>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A34:A49"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A50:A65"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A50:A65"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A34:A49"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="B46:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1832,6 +1926,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ApprovalRequested xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xsi:nil="true"/>
+    <ApprovedBy xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </ApprovedBy>
+    <Comments xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xsi:nil="true"/>
+    <Approved_x003f_ xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a">false</Approved_x003f_>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="029942aa-539e-4767-81e4-a62063a6e1cb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100695ECA461C232F4AAEC38BDBCF991C34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="59a9ea53a97323102fd6db9b998f0b5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xmlns:ns3="029942aa-539e-4767-81e4-a62063a6e1cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1df2dcb4e8f42f9041788b58686dd0b" ns2:_="" ns3:_="">
     <xsd:import namespace="b78d6d24-d6db-4d75-9c62-aa5d16939a2a"/>
@@ -2114,27 +2229,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ApprovalRequested xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xsi:nil="true"/>
-    <ApprovedBy xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </ApprovedBy>
-    <Comments xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a" xsi:nil="true"/>
-    <Approved_x003f_ xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a">false</Approved_x003f_>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b78d6d24-d6db-4d75-9c62-aa5d16939a2a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="029942aa-539e-4767-81e4-a62063a6e1cb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2145,11 +2239,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72F46C54-F7FE-4881-AE33-32A42E9027D0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDD6B012-B9AC-4751-AE85-9BF9548DF2A7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDD6B012-B9AC-4751-AE85-9BF9548DF2A7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72F46C54-F7FE-4881-AE33-32A42E9027D0}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>